<commit_message>
#812 fix testing bug for example pipeline tests
</commit_message>
<xml_diff>
--- a/src/a20_world_logic/test/test_z_examples/a23_creg1/a23_bricks.xlsx
+++ b/src/a20_world_logic/test/test_z_examples/a23_creg1/a23_bricks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\jaar\src\a20_world_logic\test\test_z_examples\a23_creg1\mud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\jaar\src\a20_world_logic\test\test_z_examples\a23_creg1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF68F2E9-9E07-4D33-9DAE-29E3E957872E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B4E255-9925-485A-BA10-B219713C19C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>